<commit_message>
Added test cases for invalid scenarios to POST/PUT Modified POM dependencies by removing selenium and webdriver dependencies
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Skills.xlsx
+++ b/src/test/resources/TestData/InputData_Skills.xlsx
@@ -4,21 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15255" windowHeight="3360"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Skills_GET" sheetId="1" r:id="rId1"/>
     <sheet name="Skills_POST" sheetId="2" r:id="rId2"/>
     <sheet name="Skills_PUT" sheetId="3" r:id="rId3"/>
     <sheet name="Skills_DELETE" sheetId="4" r:id="rId4"/>
+    <sheet name="Invalid_Key" sheetId="5" r:id="rId5"/>
+    <sheet name="Invalid_content" sheetId="6" r:id="rId6"/>
+    <sheet name="Invalid_Key_PUT" sheetId="8" r:id="rId7"/>
+    <sheet name="Invalid_content_PUT" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
+    <sheet name="Text_PUT" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:E10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
   <si>
     <t>Scenario</t>
   </si>
@@ -32,10 +37,10 @@
     <t>StatusMessage</t>
   </si>
   <si>
-    <t>GET method for Valid SkillID</t>
-  </si>
-  <si>
-    <t>GET method for inValid SkillID</t>
+    <t>GET method for an existing Skill_Id</t>
+  </si>
+  <si>
+    <t>GET method for inValid Skill_Id</t>
   </si>
   <si>
     <t>US2022</t>
@@ -44,22 +49,22 @@
     <t>Skill not found</t>
   </si>
   <si>
-    <t>GET method for Alphanumeric SkillID</t>
+    <t>GET method for Alphanumeric Skill_Id</t>
   </si>
   <si>
     <t>Java123</t>
   </si>
   <si>
-    <t>GET method for  SkillID with special character</t>
+    <t>GET method for  Skill_Id with special character</t>
   </si>
   <si>
     <t>@!#</t>
   </si>
   <si>
-    <t>GET method for  SkillID with decimal</t>
-  </si>
-  <si>
-    <t>GET method for  SkillID as blank</t>
+    <t>GET method for  Skill_Id with decimal</t>
+  </si>
+  <si>
+    <t>GET method for  Skill_Id as blank</t>
   </si>
   <si>
     <t>Skill_name</t>
@@ -68,7 +73,7 @@
     <t>POST method for Valid Skill_name</t>
   </si>
   <si>
-    <t>abcde</t>
+    <t>ccc</t>
   </si>
   <si>
     <t>Skill record successfully created</t>
@@ -152,7 +157,7 @@
     <t>To update Skill name to an already existing name</t>
   </si>
   <si>
-    <t>Python</t>
+    <t>PostgresSQL</t>
   </si>
   <si>
     <t>Failed to update-Duplicate skill name</t>
@@ -180,22 +185,61 @@
   </si>
   <si>
     <t>Failed to delete-Skill not found</t>
+  </si>
+  <si>
+    <t>User enters the Skill_id as alphanumeric.</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>Failed to delete-invalid skill id</t>
+  </si>
+  <si>
+    <t>User enters the Skill_id as decimal</t>
   </si>
   <si>
     <t xml:space="preserve">User leaves the Skill_id blank.
 </t>
   </si>
   <si>
-    <t>User enters the Skill_id as alphanumeric.</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>Failed to delete-invalid skill id</t>
-  </si>
-  <si>
-    <t>User enters the Skill_id as decimal</t>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>kill_name</t>
+  </si>
+  <si>
+    <t>POST method for InValid Key: Skill_name</t>
+  </si>
+  <si>
+    <t>Mongo</t>
+  </si>
+  <si>
+    <t>Failed to create-missing mandatory fields</t>
+  </si>
+  <si>
+    <t>POST method for InValid content</t>
+  </si>
+  <si>
+    <t>Failed to create-missing mandatory fields</t>
+  </si>
+  <si>
+    <t>ill_name</t>
+  </si>
+  <si>
+    <t>PUT method for InValid Key: Skill_name</t>
+  </si>
+  <si>
+    <t>POST method for improper JSON format request Skill_name</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Improper JSON format</t>
+  </si>
+  <si>
+    <t>PUT method for improper JSON format request Skill_name</t>
   </si>
 </sst>
 </file>
@@ -203,14 +247,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0;[Red]0"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +266,17 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -234,32 +289,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,6 +316,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,39 +388,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,62 +418,25 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -403,6 +453,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -415,7 +519,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,96 +591,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -529,61 +633,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,56 +662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -681,7 +681,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,6 +703,56 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -714,157 +764,182 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -872,56 +947,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1248,8 +1310,8 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -1261,32 +1323,32 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -1300,7 +1362,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -1314,7 +1376,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -1328,7 +1390,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B6">
@@ -1342,7 +1404,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C7">
@@ -1350,6 +1412,63 @@
       </c>
       <c r="D7" t="s">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="29.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="11.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="13.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="30.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="63" customHeight="1" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1364,57 +1483,57 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="23.7142857142857" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.7142857142857" style="15" customWidth="1"/>
+    <col min="2" max="2" width="23.7142857142857" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17.7142857142857" style="6" customWidth="1"/>
     <col min="4" max="4" width="12.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="53.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="11">
-        <v>51</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="5">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D2">
         <v>201</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D3">
@@ -1425,10 +1544,10 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="25">
         <v>1000</v>
       </c>
       <c r="D4">
@@ -1439,10 +1558,10 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D5">
@@ -1453,10 +1572,10 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D6">
@@ -1467,11 +1586,11 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B7"/>
-      <c r="C7" s="20"/>
+      <c r="C7" s="24"/>
       <c r="D7">
         <v>400</v>
       </c>
@@ -1480,10 +1599,10 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D8">
@@ -1497,10 +1616,10 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="26">
         <v>19.03</v>
       </c>
       <c r="D9">
@@ -1524,184 +1643,184 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="20.4285714285714" style="11" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" style="11" customWidth="1"/>
-    <col min="4" max="4" width="15.4285714285714" style="11" customWidth="1"/>
+    <col min="2" max="2" width="20.4285714285714" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.8571428571429" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.4285714285714" style="5" customWidth="1"/>
     <col min="5" max="5" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="14">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="14">
         <v>201</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="20" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="14">
         <v>2022</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="14">
         <v>404</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="14">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="14">
         <v>400</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="14">
         <v>400</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="14">
         <v>404</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="14">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="14">
         <v>400</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="14">
         <v>456</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="14">
         <v>400</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="14">
         <v>14</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="14">
         <v>2.3</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="14">
         <v>400</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="14">
         <v>17</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="14">
         <v>400</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="19" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1716,98 +1835,371 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="43.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="14.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="33.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="14.5714285714286" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.5714285714286" style="5" customWidth="1"/>
+    <col min="4" max="4" width="33.1428571428571" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="14">
+        <v>13</v>
+      </c>
+      <c r="C2" s="14">
+        <v>200</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2345</v>
+      </c>
+      <c r="C3" s="14">
+        <v>404</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="14">
+        <v>404</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="14">
+        <v>404</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" ht="25.5" spans="1:4">
+      <c r="A6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="14">
+        <v>404</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="38.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="18.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="20.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="39.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="12.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="20.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="17.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="45" spans="1:5">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="38.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="37.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="34.8571428571429" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.2857142857143" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="20.4285714285714" style="5" customWidth="1"/>
+    <col min="5" max="5" width="28.8571428571429" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" ht="55" customHeight="1" spans="1:5">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>400</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="$A1:$XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="29.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="5">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5">
-        <v>200</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2345</v>
-      </c>
-      <c r="C3" s="5">
-        <v>404</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" ht="25.5" spans="1:4">
-      <c r="A4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5">
-        <v>404</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="5">
-        <v>404</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>404</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading with changes in Skills feature file and input data!!
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Skills.xlsx
+++ b/src/test/resources/TestData/InputData_Skills.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" activeTab="3"/>
+    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Skills_GET" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Invalid_content" sheetId="6" r:id="rId6"/>
     <sheet name="Invalid_Key_PUT" sheetId="8" r:id="rId7"/>
     <sheet name="Invalid_content_PUT" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
+    <sheet name="Text_POST" sheetId="10" r:id="rId9"/>
     <sheet name="Text_PUT" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
   <si>
     <t>Scenario</t>
   </si>
@@ -73,7 +73,7 @@
     <t>POST method for Valid Skill_name</t>
   </si>
   <si>
-    <t>ccc</t>
+    <t>Cassanda</t>
   </si>
   <si>
     <t>Skill record successfully created</t>
@@ -112,10 +112,7 @@
     <t>POST method for Alphanumeric Skill_name</t>
   </si>
   <si>
-    <t>VCS123</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>V5</t>
   </si>
   <si>
     <t>POST method for  Skill_name with decimal</t>
@@ -124,7 +121,7 @@
     <t>Update an existing skill record</t>
   </si>
   <si>
-    <t>Playing</t>
+    <t>Oracle</t>
   </si>
   <si>
     <t>Skill record successfully updated</t>
@@ -157,7 +154,7 @@
     <t>To update Skill name to an already existing name</t>
   </si>
   <si>
-    <t>PostgresSQL</t>
+    <t>RDBMS</t>
   </si>
   <si>
     <t>Failed to update-Duplicate skill name</t>
@@ -206,7 +203,7 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t>kill_name</t>
+    <t>skill_name</t>
   </si>
   <si>
     <t>POST method for InValid Key: Skill_name</t>
@@ -221,13 +218,13 @@
     <t>POST method for InValid content</t>
   </si>
   <si>
-    <t>Failed to create-missing mandatory fields</t>
-  </si>
-  <si>
     <t>ill_name</t>
   </si>
   <si>
     <t>PUT method for InValid Key: Skill_name</t>
+  </si>
+  <si>
+    <t>Failed to update-missing mandatory fields</t>
   </si>
   <si>
     <t>POST method for improper JSON format request Skill_name</t>
@@ -249,9 +246,9 @@
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0;[Red]0"/>
     <numFmt numFmtId="179" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="25">
@@ -294,20 +291,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -317,7 +300,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,14 +337,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -380,20 +378,19 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -402,7 +399,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -425,7 +422,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,187 +450,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +655,17 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,17 +711,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -736,6 +733,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -750,24 +756,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -782,31 +779,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -815,101 +812,101 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -983,12 +980,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,106 +1309,108 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="47.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="13.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="27.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="13.8571428571429" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27.2857142857143" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="14">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="14">
         <v>200</v>
       </c>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="14">
         <v>404</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="14">
         <v>404</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="14">
         <v>404</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="14">
         <v>1.25</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="14">
         <v>404</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14">
         <v>404</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1426,15 +1426,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A1" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="29.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="11.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="13.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="30.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="29.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.4285714285714" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
@@ -1456,19 +1456,19 @@
     </row>
     <row r="2" ht="63" customHeight="1" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="5">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2">
         <v>400</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1480,13 +1480,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="23.7142857142857" style="5" customWidth="1"/>
@@ -1517,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="5">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -1533,6 +1533,7 @@
       <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="B3"/>
       <c r="C3" s="24" t="s">
         <v>19</v>
       </c>
@@ -1547,6 +1548,7 @@
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="B4"/>
       <c r="C4" s="25">
         <v>1000</v>
       </c>
@@ -1598,10 +1600,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="B8">
+        <v>68</v>
+      </c>
       <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
@@ -1611,25 +1616,22 @@
       <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="9" t="s">
-        <v>31</v>
+      <c r="B9">
+        <v>69</v>
       </c>
       <c r="C9" s="26">
-        <v>19.03</v>
+        <v>1.7</v>
       </c>
       <c r="D9">
         <v>400</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1643,8 +1645,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1675,30 +1677,30 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="14">
+        <v>4</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="14">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="D2" s="14">
         <v>201</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="14">
         <v>2022</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="14">
         <v>404</v>
@@ -1709,7 +1711,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="14">
         <v>3</v>
@@ -1721,33 +1723,33 @@
         <v>400</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="14">
         <v>400</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="14">
         <v>404</v>
@@ -1758,24 +1760,24 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="14">
         <v>8</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="14">
         <v>400</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="14">
         <v>3</v>
@@ -1787,12 +1789,12 @@
         <v>400</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="14">
         <v>14</v>
@@ -1804,24 +1806,24 @@
         <v>400</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="14">
         <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="14">
         <v>400</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1835,16 +1837,16 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="43.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="14.5714285714286" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.5714285714286" style="5" customWidth="1"/>
-    <col min="4" max="4" width="33.1428571428571" style="5" customWidth="1"/>
+    <col min="1" max="1" width="43.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5714285714286" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5714285714286" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.1428571428571" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
@@ -1863,7 +1865,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="14">
         <v>13</v>
@@ -1872,12 +1874,12 @@
         <v>200</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="14">
         <v>2345</v>
@@ -1886,26 +1888,26 @@
         <v>404</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="C4" s="14">
         <v>404</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="14">
         <v>1.2</v>
@@ -1914,21 +1916,21 @@
         <v>404</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" ht="25.5" spans="1:4">
       <c r="A6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="C6" s="14">
         <v>404</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1943,7 +1945,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1963,7 +1965,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1974,16 +1976,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
         <v>62</v>
-      </c>
-      <c r="D2">
-        <v>400</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1998,16 +2000,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="12.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="20.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="17.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.8571428571429" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
@@ -2027,13 +2029,13 @@
     </row>
     <row r="2" ht="45" spans="1:5">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2048,7 +2050,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -2065,7 +2067,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2076,19 +2078,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2102,8 +2104,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -2134,7 +2136,7 @@
     </row>
     <row r="2" ht="55" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5">
         <v>3</v>
@@ -2143,7 +2145,7 @@
         <v>400</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2155,51 +2157,57 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="$A1:$XFD2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="20.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="29.5714285714286" customWidth="1"/>
+    <col min="1" max="2" width="42.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="13.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="20.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="29.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="30" spans="1:5">
+    <row r="2" ht="30" spans="1:6">
       <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="E2">
+        <v>400</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="D2">
-        <v>400</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed constants & added authorization testcases in all API endPoints
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Skills.xlsx
+++ b/src/test/resources/TestData/InputData_Skills.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6D947CCD-040F-4181-ABF8-36C7E85D7A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="19836" windowHeight="11220" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills_GET" sheetId="1" r:id="rId1"/>
@@ -15,15 +16,17 @@
     <sheet name="Invalid_content" sheetId="6" r:id="rId6"/>
     <sheet name="Invalid_Key_PUT" sheetId="8" r:id="rId7"/>
     <sheet name="Invalid_content_PUT" sheetId="9" r:id="rId8"/>
-    <sheet name="Text_POST" sheetId="10" r:id="rId9"/>
-    <sheet name="Text_PUT" sheetId="11" r:id="rId10"/>
+    <sheet name="Skills_Authorization" sheetId="12" r:id="rId9"/>
+    <sheet name="Text_POST" sheetId="10" r:id="rId10"/>
+    <sheet name="Text_PUT" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q3"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
   <si>
     <t>Scenario</t>
   </si>
@@ -237,21 +240,53 @@
   </si>
   <si>
     <t>PUT method for improper JSON format request Skill_name</t>
+  </si>
+  <si>
+    <t>SCENARIO</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>To Check Authorization without providing username and password</t>
+  </si>
+  <si>
+    <t>Unauthorized Access</t>
+  </si>
+  <si>
+    <t>To Check Authorization with invalid username and correct password</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>2xx@Success</t>
+  </si>
+  <si>
+    <t>To Check Authorization with valid username and invalid password</t>
+  </si>
+  <si>
+    <t>APIPROCESSING</t>
+  </si>
+  <si>
+    <t>New@2022</t>
+  </si>
+  <si>
+    <t>To Check Authorization with valid username and password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0;[Red]0"/>
-    <numFmt numFmtId="179" formatCode="0.00;[Red]0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,147 +330,10 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,194 +346,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -659,254 +371,30 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -980,69 +468,31 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1300,27 +750,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="47.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="13.8571428571429" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13" style="5" customWidth="1"/>
-    <col min="4" max="4" width="27.2857142857143" style="5" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.33203125" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1416,28 +866,86 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="42.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8">
+      <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2">
+        <v>400</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="63" customHeight="1" spans="1:5">
+    <row r="2" spans="1:5" ht="63" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -1473,29 +981,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1"/>
-    <col min="2" max="2" width="23.7142857142857" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.7142857142857" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="53.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="52" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.6640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="53.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="5">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -1605,7 +1111,7 @@
         <v>28</v>
       </c>
       <c r="B8">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>29</v>
@@ -1622,7 +1128,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C9" s="26">
         <v>1.7</v>
@@ -1636,29 +1142,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="20.4285714285714" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" style="5" customWidth="1"/>
-    <col min="4" max="4" width="15.4285714285714" style="5" customWidth="1"/>
-    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.44140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.88671875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="48" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1800,7 +1304,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="14">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D9" s="14">
         <v>400</v>
@@ -1828,28 +1332,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5714285714286" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5714285714286" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.1428571428571" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="43.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.109375" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1421,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" ht="25.5" spans="1:4">
+    <row r="6" spans="1:4" ht="26.4">
       <c r="A6" s="18" t="s">
         <v>57</v>
       </c>
@@ -1935,29 +1437,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="18.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="20.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="39.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1990,29 +1490,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.4285714285714" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1428571428571" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +1525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="45" spans="1:5">
+    <row r="2" spans="1:5" ht="43.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2040,26 +1538,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="37.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="38.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2095,29 +1591,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.8571428571429" style="5" customWidth="1"/>
-    <col min="2" max="2" width="19.2857142857143" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="20.4285714285714" style="5" customWidth="1"/>
-    <col min="5" max="5" width="28.8571428571429" style="5" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.33203125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.44140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.88671875" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2134,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="55" customHeight="1" spans="1:5">
+    <row r="2" spans="1:5" ht="55.05" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>63</v>
       </c>
@@ -2150,68 +1644,109 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831B9A0F-C58A-44D6-A65A-90ED40335AB0}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="2" width="42.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="13.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="20.1428571428571" customWidth="1"/>
-    <col min="6" max="6" width="29.5714285714286" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A1" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" ht="30" spans="1:6">
-      <c r="A2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2">
-        <v>400</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" spans="1:6" ht="115.8" thickBot="1">
+      <c r="A2" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29">
+        <v>401</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="115.8" thickBot="1">
+      <c r="A3" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="29">
+        <v>401</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:6" ht="115.8" thickBot="1">
+      <c r="A4" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="29">
+        <v>401</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" spans="1:6" ht="101.4" thickBot="1">
+      <c r="A5" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="29">
+        <v>200</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{7F2CBD41-ED7D-45A7-96FC-B0B9E6BA4F21}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{8B3CB650-9738-493C-B683-5061501033B7}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{AACBE4F5-FFCA-4AC9-8CA0-12DB2E481EB0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed inputs in the excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Skills.xlsx
+++ b/src/test/resources/TestData/InputData_Skills.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DAFBC808-E665-4AA9-A2F4-F74D72B16FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{44511A7D-1EF3-47C6-A938-1E7CE2B0839A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8388" yWindow="480" windowWidth="19860" windowHeight="13224" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="0" windowWidth="19956" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills_GET" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Text_PUT" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F9"/>
+  <oleSize ref="A4:E11"/>
 </workbook>
 </file>
 
@@ -759,7 +759,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1023,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="5">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>16</v>
@@ -1111,16 +1111,16 @@
         <v>28</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D8">
-        <v>400</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
+        <v>201</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1128,7 +1128,7 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C9" s="26">
         <v>1.7</v>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1340,7 +1340,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1370,7 +1370,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="14">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C2" s="14">
         <v>200</v>

</xml_diff>